<commit_message>
Finalized the neural network training code with stable convergence. added files for the DCAM SDK for the camera control and image acquisition
</commit_message>
<xml_diff>
--- a/Neural Network Training/fc2_weights.xlsx
+++ b/Neural Network Training/fc2_weights.xlsx
@@ -512,772 +512,772 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.008492979221045971</v>
+        <v>0.00501302070915699</v>
       </c>
       <c r="B2" t="n">
-        <v>0.00362068135291338</v>
+        <v>0.00814660731703043</v>
       </c>
       <c r="C2" t="n">
-        <v>0.006437303964048624</v>
+        <v>0.003059754613786936</v>
       </c>
       <c r="D2" t="n">
-        <v>0.009054232388734818</v>
+        <v>0.002897983649745584</v>
       </c>
       <c r="E2" t="n">
-        <v>0.00212965183891356</v>
+        <v>0.005657898262143135</v>
       </c>
       <c r="F2" t="n">
-        <v>0.003284643869847059</v>
+        <v>0.005501571577042341</v>
       </c>
       <c r="G2" t="n">
-        <v>0.006369887851178646</v>
+        <v>0.004694610368460417</v>
       </c>
       <c r="H2" t="n">
-        <v>0.003380427602678537</v>
+        <v>0.005362608935683966</v>
       </c>
       <c r="I2" t="n">
-        <v>0.006126630119979382</v>
+        <v>0.006804796401411295</v>
       </c>
       <c r="J2" t="n">
-        <v>0.003857379080727696</v>
+        <v>0.008153902366757393</v>
       </c>
       <c r="K2" t="n">
-        <v>0.004801219794899225</v>
+        <v>0.002594442805275321</v>
       </c>
       <c r="L2" t="n">
-        <v>0.002920944010838866</v>
+        <v>0.005813659634441137</v>
       </c>
       <c r="M2" t="n">
-        <v>0.002455791691318154</v>
+        <v>0.005747523158788681</v>
       </c>
       <c r="N2" t="n">
-        <v>0.005867439787834883</v>
+        <v>0.005137752275913954</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0050089992582798</v>
+        <v>0.003230901435017586</v>
       </c>
       <c r="P2" t="n">
-        <v>0.006425761617720127</v>
+        <v>0.006157819647341967</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.006706180516630411</v>
+        <v>0.00591227924451232</v>
       </c>
       <c r="R2" t="n">
-        <v>0.00274887471459806</v>
+        <v>0.006390079855918884</v>
       </c>
       <c r="S2" t="n">
-        <v>0.002141269156709313</v>
+        <v>0.005798114463686943</v>
       </c>
       <c r="T2" t="n">
-        <v>0.006782582029700279</v>
+        <v>0.005869252141565084</v>
       </c>
       <c r="U2" t="n">
-        <v>0.01260573323816061</v>
+        <v>0.003565953113138676</v>
       </c>
       <c r="V2" t="n">
-        <v>0.004237488843500614</v>
+        <v>0.004250727593898773</v>
       </c>
       <c r="W2" t="n">
-        <v>0.00505707086995244</v>
+        <v>0.00488096009939909</v>
       </c>
       <c r="X2" t="n">
-        <v>0.002592868637293577</v>
+        <v>0.005659686401486397</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.002231331542134285</v>
+        <v>0.008414621464908123</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.002916996600106359</v>
+        <v>0.004365543369203806</v>
       </c>
       <c r="B3" t="n">
-        <v>0.003832924412563443</v>
+        <v>0.003002271754667163</v>
       </c>
       <c r="C3" t="n">
-        <v>0.001384301926009357</v>
+        <v>0.008729238994419575</v>
       </c>
       <c r="D3" t="n">
-        <v>0.002352589974179864</v>
+        <v>0.002648903988301754</v>
       </c>
       <c r="E3" t="n">
-        <v>0.005690830294042826</v>
+        <v>0.005462262779474258</v>
       </c>
       <c r="F3" t="n">
-        <v>0.006154621485620737</v>
+        <v>0.006776066496968269</v>
       </c>
       <c r="G3" t="n">
-        <v>0.001628546859137714</v>
+        <v>0.002805326599627733</v>
       </c>
       <c r="H3" t="n">
-        <v>0.007277361582964659</v>
+        <v>0.005176117643713951</v>
       </c>
       <c r="I3" t="n">
-        <v>0.00416305847465992</v>
+        <v>0.003131055273115635</v>
       </c>
       <c r="J3" t="n">
-        <v>0.008102742023766041</v>
+        <v>0.00597151555120945</v>
       </c>
       <c r="K3" t="n">
-        <v>0.006897289771586657</v>
+        <v>0.006347954738885164</v>
       </c>
       <c r="L3" t="n">
-        <v>0.004101295955479145</v>
+        <v>0.004453947767615318</v>
       </c>
       <c r="M3" t="n">
-        <v>0.001366169541142881</v>
+        <v>0.004268149845302105</v>
       </c>
       <c r="N3" t="n">
-        <v>0.002531429752707481</v>
+        <v>0.003263324499130249</v>
       </c>
       <c r="O3" t="n">
-        <v>0.003814884694293141</v>
+        <v>0.006000494584441185</v>
       </c>
       <c r="P3" t="n">
-        <v>0.005582849029451609</v>
+        <v>0.006398424040526152</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.004203289747238159</v>
+        <v>0.006906253285706043</v>
       </c>
       <c r="R3" t="n">
-        <v>0.005239097401499748</v>
+        <v>0.003129629651084542</v>
       </c>
       <c r="S3" t="n">
-        <v>0.006254080217331648</v>
+        <v>0.003802589373663068</v>
       </c>
       <c r="T3" t="n">
-        <v>0.004110828042030334</v>
+        <v>0.007390984334051609</v>
       </c>
       <c r="U3" t="n">
-        <v>0.007963593117892742</v>
+        <v>0.009176257066428661</v>
       </c>
       <c r="V3" t="n">
-        <v>0.008108732290565968</v>
+        <v>0.006761261727660894</v>
       </c>
       <c r="W3" t="n">
-        <v>0.005771299358457327</v>
+        <v>0.00353482342325151</v>
       </c>
       <c r="X3" t="n">
-        <v>0.006359856110066175</v>
+        <v>0.005150559823960066</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.007330000400543213</v>
+        <v>0.004146734718233347</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.009620880708098412</v>
+        <v>0.006308963987976313</v>
       </c>
       <c r="B4" t="n">
-        <v>0.003695001127198339</v>
+        <v>0.003470324911177158</v>
       </c>
       <c r="C4" t="n">
-        <v>0.004610947333276272</v>
+        <v>0.003853089641779661</v>
       </c>
       <c r="D4" t="n">
-        <v>0.008140190504491329</v>
+        <v>0.006367854308336973</v>
       </c>
       <c r="E4" t="n">
-        <v>0.004755957517772913</v>
+        <v>0.004535463638603687</v>
       </c>
       <c r="F4" t="n">
-        <v>0.003950785379856825</v>
+        <v>0.005181795917451382</v>
       </c>
       <c r="G4" t="n">
-        <v>0.003907552920281887</v>
+        <v>0.005998871754854918</v>
       </c>
       <c r="H4" t="n">
-        <v>0.005734007339924574</v>
+        <v>0.005754152312874794</v>
       </c>
       <c r="I4" t="n">
-        <v>0.005969149991869926</v>
+        <v>0.004307739902287722</v>
       </c>
       <c r="J4" t="n">
-        <v>0.003924824297428131</v>
+        <v>0.007268127519637346</v>
       </c>
       <c r="K4" t="n">
-        <v>0.006693470757454634</v>
+        <v>0.004070294089615345</v>
       </c>
       <c r="L4" t="n">
-        <v>0.004755387548357248</v>
+        <v>0.004683109931647778</v>
       </c>
       <c r="M4" t="n">
-        <v>0.007961826398968697</v>
+        <v>0.009245186112821102</v>
       </c>
       <c r="N4" t="n">
-        <v>0.003589045954868197</v>
+        <v>0.004130790010094643</v>
       </c>
       <c r="O4" t="n">
-        <v>0.004182867240160704</v>
+        <v>0.004101778380572796</v>
       </c>
       <c r="P4" t="n">
-        <v>0.004432483110576868</v>
+        <v>0.006526199635118246</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.006297688465565443</v>
+        <v>0.006083562504500151</v>
       </c>
       <c r="R4" t="n">
-        <v>0.005636157002300024</v>
+        <v>0.005379387177526951</v>
       </c>
       <c r="S4" t="n">
-        <v>0.005336326081305742</v>
+        <v>0.004784940741956234</v>
       </c>
       <c r="T4" t="n">
-        <v>0.004406434018164873</v>
+        <v>0.004703457467257977</v>
       </c>
       <c r="U4" t="n">
-        <v>0.004995405673980713</v>
+        <v>0.00644352613016963</v>
       </c>
       <c r="V4" t="n">
-        <v>0.004837384447455406</v>
+        <v>0.006363909691572189</v>
       </c>
       <c r="W4" t="n">
-        <v>0.004530458245426416</v>
+        <v>0.003547857515513897</v>
       </c>
       <c r="X4" t="n">
-        <v>0.005192209966480732</v>
+        <v>0.008134170435369015</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.004052337724715471</v>
+        <v>0.00834331288933754</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.009847936220467091</v>
+        <v>0.006133642513304949</v>
       </c>
       <c r="B5" t="n">
-        <v>0.005167496856302023</v>
+        <v>0.003300410462543368</v>
       </c>
       <c r="C5" t="n">
-        <v>0.005243778228759766</v>
+        <v>0.00394603842869401</v>
       </c>
       <c r="D5" t="n">
-        <v>0.006576780695468187</v>
+        <v>0.005743989255279303</v>
       </c>
       <c r="E5" t="n">
-        <v>0.003918627742677927</v>
+        <v>0.003768580965697765</v>
       </c>
       <c r="F5" t="n">
-        <v>0.004268740303814411</v>
+        <v>0.006243803538382053</v>
       </c>
       <c r="G5" t="n">
-        <v>0.002494220854714513</v>
+        <v>0.005844675470143557</v>
       </c>
       <c r="H5" t="n">
-        <v>0.005057975184172392</v>
+        <v>0.00574724655598402</v>
       </c>
       <c r="I5" t="n">
-        <v>0.005537055898457766</v>
+        <v>0.003514606971293688</v>
       </c>
       <c r="J5" t="n">
-        <v>0.003097545588389039</v>
+        <v>0.006739668548107147</v>
       </c>
       <c r="K5" t="n">
-        <v>0.006874528713524342</v>
+        <v>0.005229535978287458</v>
       </c>
       <c r="L5" t="n">
-        <v>0.004338640253990889</v>
+        <v>0.005412743426859379</v>
       </c>
       <c r="M5" t="n">
-        <v>0.008294559083878994</v>
+        <v>0.01014078035950661</v>
       </c>
       <c r="N5" t="n">
-        <v>0.00311516597867012</v>
+        <v>0.003004990052431822</v>
       </c>
       <c r="O5" t="n">
-        <v>0.004696825053542852</v>
+        <v>0.004074451513588428</v>
       </c>
       <c r="P5" t="n">
-        <v>0.005547598004341125</v>
+        <v>0.004780580755323172</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.005039059557020664</v>
+        <v>0.006215421482920647</v>
       </c>
       <c r="R5" t="n">
-        <v>0.005441686138510704</v>
+        <v>0.004451232962310314</v>
       </c>
       <c r="S5" t="n">
-        <v>0.006561259273439646</v>
+        <v>0.005480075255036354</v>
       </c>
       <c r="T5" t="n">
-        <v>0.006326159462332726</v>
+        <v>0.003980256617069244</v>
       </c>
       <c r="U5" t="n">
-        <v>0.003968133591115475</v>
+        <v>0.006901501677930355</v>
       </c>
       <c r="V5" t="n">
-        <v>0.004676849581301212</v>
+        <v>0.006819932721555233</v>
       </c>
       <c r="W5" t="n">
-        <v>0.004874975420534611</v>
+        <v>0.004528035875409842</v>
       </c>
       <c r="X5" t="n">
-        <v>0.005553873721510172</v>
+        <v>0.005348443053662777</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.003605420934036374</v>
+        <v>0.007890861481428146</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.003960580099374056</v>
+        <v>0.004410427063703537</v>
       </c>
       <c r="B6" t="n">
-        <v>0.006941675208508968</v>
+        <v>0.00779814412817359</v>
       </c>
       <c r="C6" t="n">
-        <v>0.006911759730428457</v>
+        <v>0.006623660679906607</v>
       </c>
       <c r="D6" t="n">
-        <v>0.002464149612933397</v>
+        <v>0.007550285197794437</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00634292047470808</v>
+        <v>0.005634637549519539</v>
       </c>
       <c r="F6" t="n">
-        <v>0.003654959611594677</v>
+        <v>0.005063801538199186</v>
       </c>
       <c r="G6" t="n">
-        <v>0.006476532202214003</v>
+        <v>0.006502262782305479</v>
       </c>
       <c r="H6" t="n">
-        <v>0.006531101651489735</v>
+        <v>0.00424187583848834</v>
       </c>
       <c r="I6" t="n">
-        <v>0.003790761344134808</v>
+        <v>0.007122132927179337</v>
       </c>
       <c r="J6" t="n">
-        <v>0.005548539105802774</v>
+        <v>0.003072797553613782</v>
       </c>
       <c r="K6" t="n">
-        <v>0.003341637318953872</v>
+        <v>0.007352421525865793</v>
       </c>
       <c r="L6" t="n">
-        <v>0.005890627391636372</v>
+        <v>0.004451698157936335</v>
       </c>
       <c r="M6" t="n">
-        <v>0.006544155534356833</v>
+        <v>0.005436756648123264</v>
       </c>
       <c r="N6" t="n">
-        <v>0.009102192707359791</v>
+        <v>0.00618754280731082</v>
       </c>
       <c r="O6" t="n">
-        <v>0.006487229838967323</v>
+        <v>0.004703857935965061</v>
       </c>
       <c r="P6" t="n">
-        <v>0.003195053897798061</v>
+        <v>0.00300655048340559</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.005167052615433931</v>
+        <v>0.004534672480076551</v>
       </c>
       <c r="R6" t="n">
-        <v>0.005206099711358547</v>
+        <v>0.002537994645535946</v>
       </c>
       <c r="S6" t="n">
-        <v>0.005023769102990627</v>
+        <v>0.003627720521762967</v>
       </c>
       <c r="T6" t="n">
-        <v>0.007887132465839386</v>
+        <v>0.002113222377374768</v>
       </c>
       <c r="U6" t="n">
-        <v>0.005467480979859829</v>
+        <v>0.004742089658975601</v>
       </c>
       <c r="V6" t="n">
-        <v>0.004009482450783253</v>
+        <v>0.002979620359838009</v>
       </c>
       <c r="W6" t="n">
-        <v>0.003376860404387116</v>
+        <v>0.007176556624472141</v>
       </c>
       <c r="X6" t="n">
-        <v>0.006475052796304226</v>
+        <v>0.00738568278029561</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.009018049575388432</v>
+        <v>0.006571737118065357</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.007429352030158043</v>
+        <v>0.008051042445003986</v>
       </c>
       <c r="B7" t="n">
-        <v>0.00370287848636508</v>
+        <v>0.002713868394494057</v>
       </c>
       <c r="C7" t="n">
-        <v>0.003965681418776512</v>
+        <v>0.004864039365202188</v>
       </c>
       <c r="D7" t="n">
-        <v>0.006964944303035736</v>
+        <v>0.005956981796771288</v>
       </c>
       <c r="E7" t="n">
-        <v>0.004865209572017193</v>
+        <v>0.005263557657599449</v>
       </c>
       <c r="F7" t="n">
-        <v>0.004478021990507841</v>
+        <v>0.005281328689306974</v>
       </c>
       <c r="G7" t="n">
-        <v>0.003814198542386293</v>
+        <v>0.00481819175183773</v>
       </c>
       <c r="H7" t="n">
-        <v>0.005362205673009157</v>
+        <v>0.006112782284617424</v>
       </c>
       <c r="I7" t="n">
-        <v>0.006488274782896042</v>
+        <v>0.003655838780105114</v>
       </c>
       <c r="J7" t="n">
-        <v>0.003443930763751268</v>
+        <v>0.006293738726526499</v>
       </c>
       <c r="K7" t="n">
-        <v>0.006066532339900732</v>
+        <v>0.004169346299022436</v>
       </c>
       <c r="L7" t="n">
-        <v>0.004317558836191893</v>
+        <v>0.004085661377757788</v>
       </c>
       <c r="M7" t="n">
-        <v>0.00955986138433218</v>
+        <v>0.01051744911819696</v>
       </c>
       <c r="N7" t="n">
-        <v>0.004128113854676485</v>
+        <v>0.004331423435360193</v>
       </c>
       <c r="O7" t="n">
-        <v>0.004567513708025217</v>
+        <v>0.003750816220417619</v>
       </c>
       <c r="P7" t="n">
-        <v>0.005576318129897118</v>
+        <v>0.004460667259991169</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.007811514660716057</v>
+        <v>0.006027753930538893</v>
       </c>
       <c r="R7" t="n">
-        <v>0.005209148861467838</v>
+        <v>0.005026270169764757</v>
       </c>
       <c r="S7" t="n">
-        <v>0.005799239967018366</v>
+        <v>0.005929835606366396</v>
       </c>
       <c r="T7" t="n">
-        <v>0.006715919356793165</v>
+        <v>0.005298939533531666</v>
       </c>
       <c r="U7" t="n">
-        <v>0.003501987550407648</v>
+        <v>0.005623708479106426</v>
       </c>
       <c r="V7" t="n">
-        <v>0.0050879274494946</v>
+        <v>0.005877712741494179</v>
       </c>
       <c r="W7" t="n">
-        <v>0.004373777192085981</v>
+        <v>0.005189474672079086</v>
       </c>
       <c r="X7" t="n">
-        <v>0.004273742437362671</v>
+        <v>0.006611165590584278</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.005484662484377623</v>
+        <v>0.008730988949537277</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.00331891281530261</v>
+        <v>0.003867179853841662</v>
       </c>
       <c r="B8" t="n">
-        <v>0.002213827101513743</v>
+        <v>0.008006484247744083</v>
       </c>
       <c r="C8" t="n">
-        <v>0.006059290375560522</v>
+        <v>0.005242900922894478</v>
       </c>
       <c r="D8" t="n">
-        <v>0.009152090176939964</v>
+        <v>0.005175203550606966</v>
       </c>
       <c r="E8" t="n">
-        <v>0.004461093805730343</v>
+        <v>0.004976089112460613</v>
       </c>
       <c r="F8" t="n">
-        <v>0.003111655823886395</v>
+        <v>0.003408142132684588</v>
       </c>
       <c r="G8" t="n">
-        <v>0.004208730533719063</v>
+        <v>0.004289048723876476</v>
       </c>
       <c r="H8" t="n">
-        <v>0.005356343928724527</v>
+        <v>0.005629118531942368</v>
       </c>
       <c r="I8" t="n">
-        <v>0.004211269784718752</v>
+        <v>0.006176474969834089</v>
       </c>
       <c r="J8" t="n">
-        <v>0.004937652498483658</v>
+        <v>0.006252895575016737</v>
       </c>
       <c r="K8" t="n">
-        <v>0.005055999848991632</v>
+        <v>0.002508902689442039</v>
       </c>
       <c r="L8" t="n">
-        <v>0.004884679336100817</v>
+        <v>0.003786151297390461</v>
       </c>
       <c r="M8" t="n">
-        <v>0.004515667911618948</v>
+        <v>0.006323164794594049</v>
       </c>
       <c r="N8" t="n">
-        <v>0.00548197329044342</v>
+        <v>0.004978656768798828</v>
       </c>
       <c r="O8" t="n">
-        <v>0.005163650959730148</v>
+        <v>0.00298779271543026</v>
       </c>
       <c r="P8" t="n">
-        <v>0.006389390211552382</v>
+        <v>0.006444219034165144</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.005759512539952993</v>
+        <v>0.006180702243000269</v>
       </c>
       <c r="R8" t="n">
-        <v>0.006095075979828835</v>
+        <v>0.007692439947277308</v>
       </c>
       <c r="S8" t="n">
-        <v>0.005014824215322733</v>
+        <v>0.003253122325986624</v>
       </c>
       <c r="T8" t="n">
-        <v>0.008908134885132313</v>
+        <v>0.00339067867025733</v>
       </c>
       <c r="U8" t="n">
-        <v>0.008132253773510456</v>
+        <v>0.00971576850861311</v>
       </c>
       <c r="V8" t="n">
-        <v>0.004093226511031389</v>
+        <v>0.004227834288030863</v>
       </c>
       <c r="W8" t="n">
-        <v>0.003056567395105958</v>
+        <v>0.005751709453761578</v>
       </c>
       <c r="X8" t="n">
-        <v>0.005493652075529099</v>
+        <v>0.006984673906117678</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.005562092177569866</v>
+        <v>0.008531908504664898</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.009104336611926556</v>
+        <v>0.00335196522064507</v>
       </c>
       <c r="B9" t="n">
-        <v>0.00641290657222271</v>
+        <v>0.005096503533422947</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00608906801789999</v>
+        <v>0.005853068083524704</v>
       </c>
       <c r="D9" t="n">
-        <v>0.003745759837329388</v>
+        <v>0.00722826924175024</v>
       </c>
       <c r="E9" t="n">
-        <v>0.005839638877660036</v>
+        <v>0.004597851540893316</v>
       </c>
       <c r="F9" t="n">
-        <v>0.004958346951752901</v>
+        <v>0.008879720233380795</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00525329727679491</v>
+        <v>0.006701385136693716</v>
       </c>
       <c r="H9" t="n">
-        <v>0.005494478158652782</v>
+        <v>0.004337240010499954</v>
       </c>
       <c r="I9" t="n">
-        <v>0.004591630771756172</v>
+        <v>0.00409370893612504</v>
       </c>
       <c r="J9" t="n">
-        <v>0.005126351490616798</v>
+        <v>0.002434496069326997</v>
       </c>
       <c r="K9" t="n">
-        <v>0.002480108756572008</v>
+        <v>0.007868641056120396</v>
       </c>
       <c r="L9" t="n">
-        <v>0.004472492262721062</v>
+        <v>0.006213067099452019</v>
       </c>
       <c r="M9" t="n">
-        <v>0.005601185839623213</v>
+        <v>0.005902663338929415</v>
       </c>
       <c r="N9" t="n">
-        <v>0.006362756248563528</v>
+        <v>0.005171317607164383</v>
       </c>
       <c r="O9" t="n">
-        <v>0.003983221482485533</v>
+        <v>0.003585674101486802</v>
       </c>
       <c r="P9" t="n">
-        <v>0.002553371246904135</v>
+        <v>0.005281093996018171</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.007299201563000679</v>
+        <v>0.003105536568909883</v>
       </c>
       <c r="R9" t="n">
-        <v>0.006218262482434511</v>
+        <v>0.004051409661769867</v>
       </c>
       <c r="S9" t="n">
-        <v>0.006413850467652082</v>
+        <v>0.004419621080160141</v>
       </c>
       <c r="T9" t="n">
-        <v>0.004513649269938469</v>
+        <v>0.005516893696039915</v>
       </c>
       <c r="U9" t="n">
-        <v>0.009201370179653168</v>
+        <v>0.00383515446446836</v>
       </c>
       <c r="V9" t="n">
-        <v>0.003787698224186897</v>
+        <v>0.003059990936890244</v>
       </c>
       <c r="W9" t="n">
-        <v>0.003318963572382927</v>
+        <v>0.006673517636954784</v>
       </c>
       <c r="X9" t="n">
-        <v>0.005612849723547697</v>
+        <v>0.005101115442812443</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.006932842079550028</v>
+        <v>0.002331217285245657</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.006982963997870684</v>
+        <v>0.007088754326105118</v>
       </c>
       <c r="B10" t="n">
-        <v>0.004616182297468185</v>
+        <v>0.003124070819467306</v>
       </c>
       <c r="C10" t="n">
-        <v>0.005753863602876663</v>
+        <v>0.005286357365548611</v>
       </c>
       <c r="D10" t="n">
-        <v>0.005289000459015369</v>
+        <v>0.005359235685318708</v>
       </c>
       <c r="E10" t="n">
-        <v>0.004378487356007099</v>
+        <v>0.004880788270384073</v>
       </c>
       <c r="F10" t="n">
-        <v>0.004494044929742813</v>
+        <v>0.005186669062823057</v>
       </c>
       <c r="G10" t="n">
-        <v>0.003882092423737049</v>
+        <v>0.005305210128426552</v>
       </c>
       <c r="H10" t="n">
-        <v>0.005871244240552187</v>
+        <v>0.005431593861430883</v>
       </c>
       <c r="I10" t="n">
-        <v>0.005251377820968628</v>
+        <v>0.003304714569821954</v>
       </c>
       <c r="J10" t="n">
-        <v>0.005729349795728922</v>
+        <v>0.005550472997128963</v>
       </c>
       <c r="K10" t="n">
-        <v>0.005684682633727789</v>
+        <v>0.00512164318934083</v>
       </c>
       <c r="L10" t="n">
-        <v>0.004616613034158945</v>
+        <v>0.005517160054296255</v>
       </c>
       <c r="M10" t="n">
-        <v>0.01006361190229654</v>
+        <v>0.01176260784268379</v>
       </c>
       <c r="N10" t="n">
-        <v>0.005089028738439083</v>
+        <v>0.003102650865912437</v>
       </c>
       <c r="O10" t="n">
-        <v>0.005480569321662188</v>
+        <v>0.003629377344623208</v>
       </c>
       <c r="P10" t="n">
-        <v>0.006787893828004599</v>
+        <v>0.007058610208332539</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.006219224538654089</v>
+        <v>0.005452656652778387</v>
       </c>
       <c r="R10" t="n">
-        <v>0.005054318811744452</v>
+        <v>0.004044323228299618</v>
       </c>
       <c r="S10" t="n">
-        <v>0.005091202910989523</v>
+        <v>0.005615540780127048</v>
       </c>
       <c r="T10" t="n">
-        <v>0.003627945901826024</v>
+        <v>0.004124629311263561</v>
       </c>
       <c r="U10" t="n">
-        <v>0.004368897061794996</v>
+        <v>0.007373250089585781</v>
       </c>
       <c r="V10" t="n">
-        <v>0.004941982682794333</v>
+        <v>0.005820424761623144</v>
       </c>
       <c r="W10" t="n">
-        <v>0.00451720179989934</v>
+        <v>0.005193933378905058</v>
       </c>
       <c r="X10" t="n">
-        <v>0.004290666431188583</v>
+        <v>0.006184224504977465</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.007385519798845053</v>
+        <v>0.00726889306679368</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.004680142737925053</v>
+        <v>0.007318371906876564</v>
       </c>
       <c r="B11" t="n">
-        <v>0.007103907875716686</v>
+        <v>0.007070847321301699</v>
       </c>
       <c r="C11" t="n">
-        <v>0.00792858749628067</v>
+        <v>0.00534099992364645</v>
       </c>
       <c r="D11" t="n">
-        <v>0.004413905087858438</v>
+        <v>0.007490440271794796</v>
       </c>
       <c r="E11" t="n">
-        <v>0.006600326392799616</v>
+        <v>0.004221704322844744</v>
       </c>
       <c r="F11" t="n">
-        <v>0.004841083660721779</v>
+        <v>0.006587483920156956</v>
       </c>
       <c r="G11" t="n">
-        <v>0.005963161587715149</v>
+        <v>0.004509811755269766</v>
       </c>
       <c r="H11" t="n">
-        <v>0.006723488215357065</v>
+        <v>0.004629215225577354</v>
       </c>
       <c r="I11" t="n">
-        <v>0.004554969724267721</v>
+        <v>0.00452911714091897</v>
       </c>
       <c r="J11" t="n">
-        <v>0.005609605461359024</v>
+        <v>0.002607471309602261</v>
       </c>
       <c r="K11" t="n">
-        <v>0.002408425556495786</v>
+        <v>0.009102397598326206</v>
       </c>
       <c r="L11" t="n">
-        <v>0.004173201974481344</v>
+        <v>0.006418074481189251</v>
       </c>
       <c r="M11" t="n">
-        <v>0.007822753861546516</v>
+        <v>0.008383717387914658</v>
       </c>
       <c r="N11" t="n">
-        <v>0.007869793102145195</v>
+        <v>0.004875855054706335</v>
       </c>
       <c r="O11" t="n">
-        <v>0.005166671704500914</v>
+        <v>0.002563740126788616</v>
       </c>
       <c r="P11" t="n">
-        <v>0.003607009304687381</v>
+        <v>0.0049549276009202</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.006955344695597887</v>
+        <v>0.003671885002404451</v>
       </c>
       <c r="R11" t="n">
-        <v>0.005446982569992542</v>
+        <v>0.002948172623291612</v>
       </c>
       <c r="S11" t="n">
-        <v>0.005687757395207882</v>
+        <v>0.00455693481490016</v>
       </c>
       <c r="T11" t="n">
-        <v>0.005650024861097336</v>
+        <v>0.004854270722717047</v>
       </c>
       <c r="U11" t="n">
-        <v>0.004257948137819767</v>
+        <v>0.003100236412137747</v>
       </c>
       <c r="V11" t="n">
-        <v>0.003033690853044391</v>
+        <v>0.00376258697360754</v>
       </c>
       <c r="W11" t="n">
-        <v>0.004289498552680016</v>
+        <v>0.006608922965824604</v>
       </c>
       <c r="X11" t="n">
-        <v>0.005963581614196301</v>
+        <v>0.006990725174546242</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.007389029022306204</v>
+        <v>0.004472300410270691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GSW algorithm and interface working in progress
</commit_message>
<xml_diff>
--- a/Neural Network Training/fc2_weights.xlsx
+++ b/Neural Network Training/fc2_weights.xlsx
@@ -512,772 +512,772 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.00501302070915699</v>
+        <v>0.004591068718582392</v>
       </c>
       <c r="B2" t="n">
-        <v>0.00814660731703043</v>
+        <v>2.186912059783936</v>
       </c>
       <c r="C2" t="n">
-        <v>0.003059754613786936</v>
+        <v>0.005427035968750715</v>
       </c>
       <c r="D2" t="n">
-        <v>0.002897983649745584</v>
+        <v>6.246422290802002</v>
       </c>
       <c r="E2" t="n">
-        <v>0.005657898262143135</v>
+        <v>4.384115219116211</v>
       </c>
       <c r="F2" t="n">
-        <v>0.005501571577042341</v>
+        <v>3.762005805969238</v>
       </c>
       <c r="G2" t="n">
-        <v>0.004694610368460417</v>
+        <v>1.004564762115479</v>
       </c>
       <c r="H2" t="n">
-        <v>0.005362608935683966</v>
+        <v>1.314486384391785</v>
       </c>
       <c r="I2" t="n">
-        <v>0.006804796401411295</v>
+        <v>1.938299298286438</v>
       </c>
       <c r="J2" t="n">
-        <v>0.008153902366757393</v>
+        <v>3.32776141166687</v>
       </c>
       <c r="K2" t="n">
-        <v>0.002594442805275321</v>
+        <v>5.660001277923584</v>
       </c>
       <c r="L2" t="n">
-        <v>0.005813659634441137</v>
+        <v>5.990503787994385</v>
       </c>
       <c r="M2" t="n">
-        <v>0.005747523158788681</v>
+        <v>3.653046369552612</v>
       </c>
       <c r="N2" t="n">
-        <v>0.005137752275913954</v>
+        <v>0.004531692247837782</v>
       </c>
       <c r="O2" t="n">
-        <v>0.003230901435017586</v>
+        <v>2.176706075668335</v>
       </c>
       <c r="P2" t="n">
-        <v>0.006157819647341967</v>
+        <v>3.967877626419067</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.00591227924451232</v>
+        <v>0.004104952327907085</v>
       </c>
       <c r="R2" t="n">
-        <v>0.006390079855918884</v>
+        <v>2.203673601150513</v>
       </c>
       <c r="S2" t="n">
-        <v>0.005798114463686943</v>
+        <v>0.1313426792621613</v>
       </c>
       <c r="T2" t="n">
-        <v>0.005869252141565084</v>
+        <v>0.004068870097398758</v>
       </c>
       <c r="U2" t="n">
-        <v>0.003565953113138676</v>
+        <v>0.00507756182923913</v>
       </c>
       <c r="V2" t="n">
-        <v>0.004250727593898773</v>
+        <v>2.136415958404541</v>
       </c>
       <c r="W2" t="n">
-        <v>0.00488096009939909</v>
+        <v>0.004902273416519165</v>
       </c>
       <c r="X2" t="n">
-        <v>0.005659686401486397</v>
+        <v>0.004691822919994593</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.008414621464908123</v>
+        <v>1.613394618034363</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.004365543369203806</v>
+        <v>5.713008880615234</v>
       </c>
       <c r="B3" t="n">
-        <v>0.003002271754667163</v>
+        <v>0.0002102738944813609</v>
       </c>
       <c r="C3" t="n">
-        <v>0.008729238994419575</v>
+        <v>0.00244306237436831</v>
       </c>
       <c r="D3" t="n">
-        <v>0.002648903988301754</v>
+        <v>0.0006176214665174484</v>
       </c>
       <c r="E3" t="n">
-        <v>0.005462262779474258</v>
+        <v>1.905981540679932</v>
       </c>
       <c r="F3" t="n">
-        <v>0.006776066496968269</v>
+        <v>0.0005943316500633955</v>
       </c>
       <c r="G3" t="n">
-        <v>0.002805326599627733</v>
+        <v>0.001702116569504142</v>
       </c>
       <c r="H3" t="n">
-        <v>0.005176117643713951</v>
+        <v>0.003019219264388084</v>
       </c>
       <c r="I3" t="n">
-        <v>0.003131055273115635</v>
+        <v>1.835588574409485</v>
       </c>
       <c r="J3" t="n">
-        <v>0.00597151555120945</v>
+        <v>0.02475676685571671</v>
       </c>
       <c r="K3" t="n">
-        <v>0.006347954738885164</v>
+        <v>0.003329100087285042</v>
       </c>
       <c r="L3" t="n">
-        <v>0.004453947767615318</v>
+        <v>1.283533811569214</v>
       </c>
       <c r="M3" t="n">
-        <v>0.004268149845302105</v>
+        <v>0.7580472826957703</v>
       </c>
       <c r="N3" t="n">
-        <v>0.003263324499130249</v>
+        <v>0.00204353523440659</v>
       </c>
       <c r="O3" t="n">
-        <v>0.006000494584441185</v>
+        <v>0.187361404299736</v>
       </c>
       <c r="P3" t="n">
-        <v>0.006398424040526152</v>
+        <v>0.005680469796061516</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.006906253285706043</v>
+        <v>5.431578636169434</v>
       </c>
       <c r="R3" t="n">
-        <v>0.003129629651084542</v>
+        <v>0.004768955521285534</v>
       </c>
       <c r="S3" t="n">
-        <v>0.003802589373663068</v>
+        <v>0.6577330827713013</v>
       </c>
       <c r="T3" t="n">
-        <v>0.007390984334051609</v>
+        <v>6.873856544494629</v>
       </c>
       <c r="U3" t="n">
-        <v>0.009176257066428661</v>
+        <v>5.204483032226562</v>
       </c>
       <c r="V3" t="n">
-        <v>0.006761261727660894</v>
+        <v>6.632120609283447</v>
       </c>
       <c r="W3" t="n">
-        <v>0.00353482342325151</v>
+        <v>4.60166072845459</v>
       </c>
       <c r="X3" t="n">
-        <v>0.005150559823960066</v>
+        <v>6.218491077423096</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.004146734718233347</v>
+        <v>0.001210002461448312</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.006308963987976313</v>
+        <v>1.9506756067276</v>
       </c>
       <c r="B4" t="n">
-        <v>0.003470324911177158</v>
+        <v>0.004224009811878204</v>
       </c>
       <c r="C4" t="n">
-        <v>0.003853089641779661</v>
+        <v>0.01214164029806852</v>
       </c>
       <c r="D4" t="n">
-        <v>0.006367854308336973</v>
+        <v>0.01354831922799349</v>
       </c>
       <c r="E4" t="n">
-        <v>0.004535463638603687</v>
+        <v>3.908854484558105</v>
       </c>
       <c r="F4" t="n">
-        <v>0.005181795917451382</v>
+        <v>0.00608730036765337</v>
       </c>
       <c r="G4" t="n">
-        <v>0.005998871754854918</v>
+        <v>2.115115165710449</v>
       </c>
       <c r="H4" t="n">
-        <v>0.005754152312874794</v>
+        <v>8.032851219177246</v>
       </c>
       <c r="I4" t="n">
-        <v>0.004307739902287722</v>
+        <v>4.617366790771484</v>
       </c>
       <c r="J4" t="n">
-        <v>0.007268127519637346</v>
+        <v>1.840412259101868</v>
       </c>
       <c r="K4" t="n">
-        <v>0.004070294089615345</v>
+        <v>0.003356289118528366</v>
       </c>
       <c r="L4" t="n">
-        <v>0.004683109931647778</v>
+        <v>4.469799518585205</v>
       </c>
       <c r="M4" t="n">
-        <v>0.009245186112821102</v>
+        <v>5.621973991394043</v>
       </c>
       <c r="N4" t="n">
-        <v>0.004130790010094643</v>
+        <v>0.621628999710083</v>
       </c>
       <c r="O4" t="n">
-        <v>0.004101778380572796</v>
+        <v>2.20595383644104</v>
       </c>
       <c r="P4" t="n">
-        <v>0.006526199635118246</v>
+        <v>1.223170399665833</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.006083562504500151</v>
+        <v>4.591441631317139</v>
       </c>
       <c r="R4" t="n">
-        <v>0.005379387177526951</v>
+        <v>3.292394399642944</v>
       </c>
       <c r="S4" t="n">
-        <v>0.004784940741956234</v>
+        <v>0.004453139379620552</v>
       </c>
       <c r="T4" t="n">
-        <v>0.004703457467257977</v>
+        <v>0.009770682081580162</v>
       </c>
       <c r="U4" t="n">
-        <v>0.00644352613016963</v>
+        <v>0.2070891261100769</v>
       </c>
       <c r="V4" t="n">
-        <v>0.006363909691572189</v>
+        <v>0.684496283531189</v>
       </c>
       <c r="W4" t="n">
-        <v>0.003547857515513897</v>
+        <v>5.382015228271484</v>
       </c>
       <c r="X4" t="n">
-        <v>0.008134170435369015</v>
+        <v>0.8915483951568604</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.00834331288933754</v>
+        <v>0.002153449924662709</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.006133642513304949</v>
+        <v>1.461140275001526</v>
       </c>
       <c r="B5" t="n">
-        <v>0.003300410462543368</v>
+        <v>0.004304415080696344</v>
       </c>
       <c r="C5" t="n">
-        <v>0.00394603842869401</v>
+        <v>2.584566593170166</v>
       </c>
       <c r="D5" t="n">
-        <v>0.005743989255279303</v>
+        <v>0.0201956033706665</v>
       </c>
       <c r="E5" t="n">
-        <v>0.003768580965697765</v>
+        <v>3.477282285690308</v>
       </c>
       <c r="F5" t="n">
-        <v>0.006243803538382053</v>
+        <v>0.003808443201705813</v>
       </c>
       <c r="G5" t="n">
-        <v>0.005844675470143557</v>
+        <v>0.003639432601630688</v>
       </c>
       <c r="H5" t="n">
-        <v>0.00574724655598402</v>
+        <v>6.121278762817383</v>
       </c>
       <c r="I5" t="n">
-        <v>0.003514606971293688</v>
+        <v>0.003637688234448433</v>
       </c>
       <c r="J5" t="n">
-        <v>0.006739668548107147</v>
+        <v>3.464127063751221</v>
       </c>
       <c r="K5" t="n">
-        <v>0.005229535978287458</v>
+        <v>0.00824928842484951</v>
       </c>
       <c r="L5" t="n">
-        <v>0.005412743426859379</v>
+        <v>0.003916628658771515</v>
       </c>
       <c r="M5" t="n">
-        <v>0.01014078035950661</v>
+        <v>4.584489345550537</v>
       </c>
       <c r="N5" t="n">
-        <v>0.003004990052431822</v>
+        <v>1.48308253288269</v>
       </c>
       <c r="O5" t="n">
-        <v>0.004074451513588428</v>
+        <v>4.691103935241699</v>
       </c>
       <c r="P5" t="n">
-        <v>0.004780580755323172</v>
+        <v>2.149705648422241</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.006215421482920647</v>
+        <v>0.002888125367462635</v>
       </c>
       <c r="R5" t="n">
-        <v>0.004451232962310314</v>
+        <v>4.577437877655029</v>
       </c>
       <c r="S5" t="n">
-        <v>0.005480075255036354</v>
+        <v>5.123556137084961</v>
       </c>
       <c r="T5" t="n">
-        <v>0.003980256617069244</v>
+        <v>2.871350526809692</v>
       </c>
       <c r="U5" t="n">
-        <v>0.006901501677930355</v>
+        <v>3.953562259674072</v>
       </c>
       <c r="V5" t="n">
-        <v>0.006819932721555233</v>
+        <v>4.243963718414307</v>
       </c>
       <c r="W5" t="n">
-        <v>0.004528035875409842</v>
+        <v>0.003135476727038622</v>
       </c>
       <c r="X5" t="n">
-        <v>0.005348443053662777</v>
+        <v>0.5569941997528076</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.007890861481428146</v>
+        <v>0.00924244336783886</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.004410427063703537</v>
+        <v>3.410658597946167</v>
       </c>
       <c r="B6" t="n">
-        <v>0.00779814412817359</v>
+        <v>0.5193859934806824</v>
       </c>
       <c r="C6" t="n">
-        <v>0.006623660679906607</v>
+        <v>3.805002689361572</v>
       </c>
       <c r="D6" t="n">
-        <v>0.007550285197794437</v>
+        <v>6.188418388366699</v>
       </c>
       <c r="E6" t="n">
-        <v>0.005634637549519539</v>
+        <v>0.03429876640439034</v>
       </c>
       <c r="F6" t="n">
-        <v>0.005063801538199186</v>
+        <v>0.2813860177993774</v>
       </c>
       <c r="G6" t="n">
-        <v>0.006502262782305479</v>
+        <v>5.831648349761963</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00424187583848834</v>
+        <v>0.5426952242851257</v>
       </c>
       <c r="I6" t="n">
-        <v>0.007122132927179337</v>
+        <v>0.01319483108818531</v>
       </c>
       <c r="J6" t="n">
-        <v>0.003072797553613782</v>
+        <v>1.831418633460999</v>
       </c>
       <c r="K6" t="n">
-        <v>0.007352421525865793</v>
+        <v>5.579594612121582</v>
       </c>
       <c r="L6" t="n">
-        <v>0.004451698157936335</v>
+        <v>0.00465824268758297</v>
       </c>
       <c r="M6" t="n">
-        <v>0.005436756648123264</v>
+        <v>0.004029155243188143</v>
       </c>
       <c r="N6" t="n">
-        <v>0.00618754280731082</v>
+        <v>5.427706241607666</v>
       </c>
       <c r="O6" t="n">
-        <v>0.004703857935965061</v>
+        <v>1.787075757980347</v>
       </c>
       <c r="P6" t="n">
-        <v>0.00300655048340559</v>
+        <v>0.003378417575731874</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.004534672480076551</v>
+        <v>5.225881576538086</v>
       </c>
       <c r="R6" t="n">
-        <v>0.002537994645535946</v>
+        <v>0.007809703703969717</v>
       </c>
       <c r="S6" t="n">
-        <v>0.003627720521762967</v>
+        <v>0.5318001508712769</v>
       </c>
       <c r="T6" t="n">
-        <v>0.002113222377374768</v>
+        <v>0.01222683489322662</v>
       </c>
       <c r="U6" t="n">
-        <v>0.004742089658975601</v>
+        <v>1.937697172164917</v>
       </c>
       <c r="V6" t="n">
-        <v>0.002979620359838009</v>
+        <v>0.004065602086484432</v>
       </c>
       <c r="W6" t="n">
-        <v>0.007176556624472141</v>
+        <v>1.937944531440735</v>
       </c>
       <c r="X6" t="n">
-        <v>0.00738568278029561</v>
+        <v>0.0103471614420414</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.006571737118065357</v>
+        <v>5.803413391113281</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.008051042445003986</v>
+        <v>2.844599008560181</v>
       </c>
       <c r="B7" t="n">
-        <v>0.002713868394494057</v>
+        <v>4.741164207458496</v>
       </c>
       <c r="C7" t="n">
-        <v>0.004864039365202188</v>
+        <v>0.002243695314973593</v>
       </c>
       <c r="D7" t="n">
-        <v>0.005956981796771288</v>
+        <v>1.268503427505493</v>
       </c>
       <c r="E7" t="n">
-        <v>0.005263557657599449</v>
+        <v>8.398907661437988</v>
       </c>
       <c r="F7" t="n">
-        <v>0.005281328689306974</v>
+        <v>4.01053524017334</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00481819175183773</v>
+        <v>0.005037608556449413</v>
       </c>
       <c r="H7" t="n">
-        <v>0.006112782284617424</v>
+        <v>2.781199932098389</v>
       </c>
       <c r="I7" t="n">
-        <v>0.003655838780105114</v>
+        <v>0.001711501041427255</v>
       </c>
       <c r="J7" t="n">
-        <v>0.006293738726526499</v>
+        <v>0.001031458843499422</v>
       </c>
       <c r="K7" t="n">
-        <v>0.004169346299022436</v>
+        <v>2.740577936172485</v>
       </c>
       <c r="L7" t="n">
-        <v>0.004085661377757788</v>
+        <v>1.787148714065552</v>
       </c>
       <c r="M7" t="n">
-        <v>0.01051744911819696</v>
+        <v>0.4003611207008362</v>
       </c>
       <c r="N7" t="n">
-        <v>0.004331423435360193</v>
+        <v>0.005779871717095375</v>
       </c>
       <c r="O7" t="n">
-        <v>0.003750816220417619</v>
+        <v>0.001129458658397198</v>
       </c>
       <c r="P7" t="n">
-        <v>0.004460667259991169</v>
+        <v>1.951138734817505</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.006027753930538893</v>
+        <v>0.03499886021018028</v>
       </c>
       <c r="R7" t="n">
-        <v>0.005026270169764757</v>
+        <v>1.159641742706299</v>
       </c>
       <c r="S7" t="n">
-        <v>0.005929835606366396</v>
+        <v>6.422484397888184</v>
       </c>
       <c r="T7" t="n">
-        <v>0.005298939533531666</v>
+        <v>0.007131356745958328</v>
       </c>
       <c r="U7" t="n">
-        <v>0.005623708479106426</v>
+        <v>5.555715084075928</v>
       </c>
       <c r="V7" t="n">
-        <v>0.005877712741494179</v>
+        <v>1.059916973114014</v>
       </c>
       <c r="W7" t="n">
-        <v>0.005189474672079086</v>
+        <v>0.130394920706749</v>
       </c>
       <c r="X7" t="n">
-        <v>0.006611165590584278</v>
+        <v>0.008469589985907078</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.008730988949537277</v>
+        <v>5.590366363525391</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.003867179853841662</v>
+        <v>1.498386859893799</v>
       </c>
       <c r="B8" t="n">
-        <v>0.008006484247744083</v>
+        <v>0.233984500169754</v>
       </c>
       <c r="C8" t="n">
-        <v>0.005242900922894478</v>
+        <v>0.3373751044273376</v>
       </c>
       <c r="D8" t="n">
-        <v>0.005175203550606966</v>
+        <v>4.206531524658203</v>
       </c>
       <c r="E8" t="n">
-        <v>0.004976089112460613</v>
+        <v>0.0001562673423904926</v>
       </c>
       <c r="F8" t="n">
-        <v>0.003408142132684588</v>
+        <v>0.01127286721020937</v>
       </c>
       <c r="G8" t="n">
-        <v>0.004289048723876476</v>
+        <v>1.683412313461304</v>
       </c>
       <c r="H8" t="n">
-        <v>0.005629118531942368</v>
+        <v>0.001065192511305213</v>
       </c>
       <c r="I8" t="n">
-        <v>0.006176474969834089</v>
+        <v>5.496126651763916</v>
       </c>
       <c r="J8" t="n">
-        <v>0.006252895575016737</v>
+        <v>0.001083079841919243</v>
       </c>
       <c r="K8" t="n">
-        <v>0.002508902689442039</v>
+        <v>5.948645114898682</v>
       </c>
       <c r="L8" t="n">
-        <v>0.003786151297390461</v>
+        <v>5.852470874786377</v>
       </c>
       <c r="M8" t="n">
-        <v>0.006323164794594049</v>
+        <v>0.001966696232557297</v>
       </c>
       <c r="N8" t="n">
-        <v>0.004978656768798828</v>
+        <v>0.2667432427406311</v>
       </c>
       <c r="O8" t="n">
-        <v>0.00298779271543026</v>
+        <v>0.0009038528660312295</v>
       </c>
       <c r="P8" t="n">
-        <v>0.006444219034165144</v>
+        <v>0.4684150516986847</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.006180702243000269</v>
+        <v>2.199663400650024</v>
       </c>
       <c r="R8" t="n">
-        <v>0.007692439947277308</v>
+        <v>8.177361488342285</v>
       </c>
       <c r="S8" t="n">
-        <v>0.003253122325986624</v>
+        <v>0.07305580377578735</v>
       </c>
       <c r="T8" t="n">
-        <v>0.00339067867025733</v>
+        <v>0.1000940054655075</v>
       </c>
       <c r="U8" t="n">
-        <v>0.00971576850861311</v>
+        <v>0.886012852191925</v>
       </c>
       <c r="V8" t="n">
-        <v>0.004227834288030863</v>
+        <v>0.0004968990106135607</v>
       </c>
       <c r="W8" t="n">
-        <v>0.005751709453761578</v>
+        <v>5.005722999572754</v>
       </c>
       <c r="X8" t="n">
-        <v>0.006984673906117678</v>
+        <v>5.099513530731201</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.008531908504664898</v>
+        <v>4.210269927978516</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.00335196522064507</v>
+        <v>0.005901766940951347</v>
       </c>
       <c r="B9" t="n">
-        <v>0.005096503533422947</v>
+        <v>4.256443500518799</v>
       </c>
       <c r="C9" t="n">
-        <v>0.005853068083524704</v>
+        <v>5.195938110351562</v>
       </c>
       <c r="D9" t="n">
-        <v>0.00722826924175024</v>
+        <v>0.006182674318552017</v>
       </c>
       <c r="E9" t="n">
-        <v>0.004597851540893316</v>
+        <v>0.001698993495665491</v>
       </c>
       <c r="F9" t="n">
-        <v>0.008879720233380795</v>
+        <v>3.949512004852295</v>
       </c>
       <c r="G9" t="n">
-        <v>0.006701385136693716</v>
+        <v>0.3545295894145966</v>
       </c>
       <c r="H9" t="n">
-        <v>0.004337240010499954</v>
+        <v>0.8364130854606628</v>
       </c>
       <c r="I9" t="n">
-        <v>0.00409370893612504</v>
+        <v>0.09276384860277176</v>
       </c>
       <c r="J9" t="n">
-        <v>0.002434496069326997</v>
+        <v>6.77872896194458</v>
       </c>
       <c r="K9" t="n">
-        <v>0.007868641056120396</v>
+        <v>0.01233084686100483</v>
       </c>
       <c r="L9" t="n">
-        <v>0.006213067099452019</v>
+        <v>0.004123758990317583</v>
       </c>
       <c r="M9" t="n">
-        <v>0.005902663338929415</v>
+        <v>0.003267535008490086</v>
       </c>
       <c r="N9" t="n">
-        <v>0.005171317607164383</v>
+        <v>5.680654525756836</v>
       </c>
       <c r="O9" t="n">
-        <v>0.003585674101486802</v>
+        <v>7.149709224700928</v>
       </c>
       <c r="P9" t="n">
-        <v>0.005281093996018171</v>
+        <v>4.894673347473145</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.003105536568909883</v>
+        <v>0.06682708114385605</v>
       </c>
       <c r="R9" t="n">
-        <v>0.004051409661769867</v>
+        <v>0.007031361106783152</v>
       </c>
       <c r="S9" t="n">
-        <v>0.004419621080160141</v>
+        <v>0.008566330187022686</v>
       </c>
       <c r="T9" t="n">
-        <v>0.005516893696039915</v>
+        <v>0.3613593876361847</v>
       </c>
       <c r="U9" t="n">
-        <v>0.00383515446446836</v>
+        <v>0.004120903089642525</v>
       </c>
       <c r="V9" t="n">
-        <v>0.003059990936890244</v>
+        <v>7.000304222106934</v>
       </c>
       <c r="W9" t="n">
-        <v>0.006673517636954784</v>
+        <v>2.666243314743042</v>
       </c>
       <c r="X9" t="n">
-        <v>0.005101115442812443</v>
+        <v>0.01006762124598026</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.002331217285245657</v>
+        <v>0.003580531338229775</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.007088754326105118</v>
+        <v>3.255012989044189</v>
       </c>
       <c r="B10" t="n">
-        <v>0.003124070819467306</v>
+        <v>5.15381908416748</v>
       </c>
       <c r="C10" t="n">
-        <v>0.005286357365548611</v>
+        <v>2.272378206253052</v>
       </c>
       <c r="D10" t="n">
-        <v>0.005359235685318708</v>
+        <v>0.003712342819198966</v>
       </c>
       <c r="E10" t="n">
-        <v>0.004880788270384073</v>
+        <v>2.640583992004395</v>
       </c>
       <c r="F10" t="n">
-        <v>0.005186669062823057</v>
+        <v>4.243880748748779</v>
       </c>
       <c r="G10" t="n">
-        <v>0.005305210128426552</v>
+        <v>0.004041530191898346</v>
       </c>
       <c r="H10" t="n">
-        <v>0.005431593861430883</v>
+        <v>0.007993529550731182</v>
       </c>
       <c r="I10" t="n">
-        <v>0.003304714569821954</v>
+        <v>4.409947872161865</v>
       </c>
       <c r="J10" t="n">
-        <v>0.005550472997128963</v>
+        <v>2.664298295974731</v>
       </c>
       <c r="K10" t="n">
-        <v>0.00512164318934083</v>
+        <v>0.004182351287454367</v>
       </c>
       <c r="L10" t="n">
-        <v>0.005517160054296255</v>
+        <v>4.112948417663574</v>
       </c>
       <c r="M10" t="n">
-        <v>0.01176260784268379</v>
+        <v>5.114810943603516</v>
       </c>
       <c r="N10" t="n">
-        <v>0.003102650865912437</v>
+        <v>0.004202362149953842</v>
       </c>
       <c r="O10" t="n">
-        <v>0.003629377344623208</v>
+        <v>1.058089256286621</v>
       </c>
       <c r="P10" t="n">
-        <v>0.007058610208332539</v>
+        <v>0.4905550181865692</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.005452656652778387</v>
+        <v>3.316354751586914</v>
       </c>
       <c r="R10" t="n">
-        <v>0.004044323228299618</v>
+        <v>0.002530722878873348</v>
       </c>
       <c r="S10" t="n">
-        <v>0.005615540780127048</v>
+        <v>6.137276649475098</v>
       </c>
       <c r="T10" t="n">
-        <v>0.004124629311263561</v>
+        <v>0.643217146396637</v>
       </c>
       <c r="U10" t="n">
-        <v>0.007373250089585781</v>
+        <v>2.728050231933594</v>
       </c>
       <c r="V10" t="n">
-        <v>0.005820424761623144</v>
+        <v>0.002977384487167001</v>
       </c>
       <c r="W10" t="n">
-        <v>0.005193933378905058</v>
+        <v>1.678724646568298</v>
       </c>
       <c r="X10" t="n">
-        <v>0.006184224504977465</v>
+        <v>1.100385785102844</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.00726889306679368</v>
+        <v>1.058057188987732</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.007318371906876564</v>
+        <v>4.212934494018555</v>
       </c>
       <c r="B11" t="n">
-        <v>0.007070847321301699</v>
+        <v>2.952179431915283</v>
       </c>
       <c r="C11" t="n">
-        <v>0.00534099992364645</v>
+        <v>5.61153507232666</v>
       </c>
       <c r="D11" t="n">
-        <v>0.007490440271794796</v>
+        <v>3.482506990432739</v>
       </c>
       <c r="E11" t="n">
-        <v>0.004221704322844744</v>
+        <v>0.0003373771905899048</v>
       </c>
       <c r="F11" t="n">
-        <v>0.006587483920156956</v>
+        <v>3.166513681411743</v>
       </c>
       <c r="G11" t="n">
-        <v>0.004509811755269766</v>
+        <v>3.423604488372803</v>
       </c>
       <c r="H11" t="n">
-        <v>0.004629215225577354</v>
+        <v>0.0001673406222835183</v>
       </c>
       <c r="I11" t="n">
-        <v>0.00452911714091897</v>
+        <v>0.04144493117928505</v>
       </c>
       <c r="J11" t="n">
-        <v>0.002607471309602261</v>
+        <v>2.198819160461426</v>
       </c>
       <c r="K11" t="n">
-        <v>0.009102397598326206</v>
+        <v>0.00232517090626061</v>
       </c>
       <c r="L11" t="n">
-        <v>0.006418074481189251</v>
+        <v>0.0002239847090095282</v>
       </c>
       <c r="M11" t="n">
-        <v>0.008383717387914658</v>
+        <v>0.001565230544656515</v>
       </c>
       <c r="N11" t="n">
-        <v>0.004875855054706335</v>
+        <v>4.012048721313477</v>
       </c>
       <c r="O11" t="n">
-        <v>0.002563740126788616</v>
+        <v>2.243364334106445</v>
       </c>
       <c r="P11" t="n">
-        <v>0.0049549276009202</v>
+        <v>8.73178768157959</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.003671885002404451</v>
+        <v>2.383157253265381</v>
       </c>
       <c r="R11" t="n">
-        <v>0.002948172623291612</v>
+        <v>0.0007974395994096994</v>
       </c>
       <c r="S11" t="n">
-        <v>0.00455693481490016</v>
+        <v>0.0002751208376139402</v>
       </c>
       <c r="T11" t="n">
-        <v>0.004854270722717047</v>
+        <v>1.319719552993774</v>
       </c>
       <c r="U11" t="n">
-        <v>0.003100236412137747</v>
+        <v>0.9394583106040955</v>
       </c>
       <c r="V11" t="n">
-        <v>0.00376258697360754</v>
+        <v>0.003731885924935341</v>
       </c>
       <c r="W11" t="n">
-        <v>0.006608922965824604</v>
+        <v>0.01734456792473793</v>
       </c>
       <c r="X11" t="n">
-        <v>0.006990725174546242</v>
+        <v>0.004488531500101089</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.004472300410270691</v>
+        <v>5.287984848022461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GS Algorithm working in progress
</commit_message>
<xml_diff>
--- a/Neural Network Training/fc2_weights.xlsx
+++ b/Neural Network Training/fc2_weights.xlsx
@@ -512,772 +512,772 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.004591068718582392</v>
+        <v>6.850574573036283e-05</v>
       </c>
       <c r="B2" t="n">
-        <v>2.186912059783936</v>
+        <v>0.0008434053161181509</v>
       </c>
       <c r="C2" t="n">
-        <v>0.005427035968750715</v>
+        <v>8.698595621581262e-09</v>
       </c>
       <c r="D2" t="n">
-        <v>6.246422290802002</v>
+        <v>4.319526851759292e-06</v>
       </c>
       <c r="E2" t="n">
-        <v>4.384115219116211</v>
+        <v>1.770770995926287e-14</v>
       </c>
       <c r="F2" t="n">
-        <v>3.762005805969238</v>
+        <v>1.954338380016907e-08</v>
       </c>
       <c r="G2" t="n">
-        <v>1.004564762115479</v>
+        <v>2.666527507244609e-05</v>
       </c>
       <c r="H2" t="n">
-        <v>1.314486384391785</v>
+        <v>3.933255054988649e-09</v>
       </c>
       <c r="I2" t="n">
-        <v>1.938299298286438</v>
+        <v>8.556725333619397e-06</v>
       </c>
       <c r="J2" t="n">
-        <v>3.32776141166687</v>
+        <v>0.0003688785945996642</v>
       </c>
       <c r="K2" t="n">
-        <v>5.660001277923584</v>
+        <v>2.231896800708455e-08</v>
       </c>
       <c r="L2" t="n">
-        <v>5.990503787994385</v>
+        <v>1.447957043154702e-08</v>
       </c>
       <c r="M2" t="n">
-        <v>3.653046369552612</v>
+        <v>0.008960417471826077</v>
       </c>
       <c r="N2" t="n">
-        <v>0.004531692247837782</v>
+        <v>4.422629009366639e-17</v>
       </c>
       <c r="O2" t="n">
-        <v>2.176706075668335</v>
+        <v>6.479158764705062e-05</v>
       </c>
       <c r="P2" t="n">
-        <v>3.967877626419067</v>
+        <v>2.048904867990586e-08</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.004104952327907085</v>
+        <v>2.548053679163331e-08</v>
       </c>
       <c r="R2" t="n">
-        <v>2.203673601150513</v>
+        <v>1.482119937890047e-08</v>
       </c>
       <c r="S2" t="n">
-        <v>0.1313426792621613</v>
+        <v>1.880398667708505e-05</v>
       </c>
       <c r="T2" t="n">
-        <v>0.004068870097398758</v>
+        <v>6.298531843640376e-06</v>
       </c>
       <c r="U2" t="n">
-        <v>0.00507756182923913</v>
+        <v>0.002949760761111975</v>
       </c>
       <c r="V2" t="n">
-        <v>2.136415958404541</v>
+        <v>2.668303068276145e-06</v>
       </c>
       <c r="W2" t="n">
-        <v>0.004902273416519165</v>
+        <v>2.320366121466577e-08</v>
       </c>
       <c r="X2" t="n">
-        <v>0.004691822919994593</v>
+        <v>0.0004497090412769467</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.613394618034363</v>
+        <v>0.002099902601912618</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5.713008880615234</v>
+        <v>0.0002923326683230698</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0002102738944813609</v>
+        <v>0.001285611884668469</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00244306237436831</v>
+        <v>2.299433532471085e-09</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0006176214665174484</v>
+        <v>1.917597414191619e-09</v>
       </c>
       <c r="E3" t="n">
-        <v>1.905981540679932</v>
+        <v>2.475292157259e-17</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0005943316500633955</v>
+        <v>6.374432537370467e-09</v>
       </c>
       <c r="G3" t="n">
-        <v>0.001702116569504142</v>
+        <v>4.16068323829677e-05</v>
       </c>
       <c r="H3" t="n">
-        <v>0.003019219264388084</v>
+        <v>2.234758953912665e-17</v>
       </c>
       <c r="I3" t="n">
-        <v>1.835588574409485</v>
+        <v>0.0001317159330938011</v>
       </c>
       <c r="J3" t="n">
-        <v>0.02475676685571671</v>
+        <v>3.191697760485113e-05</v>
       </c>
       <c r="K3" t="n">
-        <v>0.003329100087285042</v>
+        <v>0.0005330232670530677</v>
       </c>
       <c r="L3" t="n">
-        <v>1.283533811569214</v>
+        <v>4.276933029956353e-09</v>
       </c>
       <c r="M3" t="n">
-        <v>0.7580472826957703</v>
+        <v>0.00777438236400485</v>
       </c>
       <c r="N3" t="n">
-        <v>0.00204353523440659</v>
+        <v>2.147962065056863e-17</v>
       </c>
       <c r="O3" t="n">
-        <v>0.187361404299736</v>
+        <v>7.201521384558873e-06</v>
       </c>
       <c r="P3" t="n">
-        <v>0.005680469796061516</v>
+        <v>5.514883797026748e-13</v>
       </c>
       <c r="Q3" t="n">
-        <v>5.431578636169434</v>
+        <v>2.212343641616599e-09</v>
       </c>
       <c r="R3" t="n">
-        <v>0.004768955521285534</v>
+        <v>2.145699389650632e-13</v>
       </c>
       <c r="S3" t="n">
-        <v>0.6577330827713013</v>
+        <v>0.0002137597184628248</v>
       </c>
       <c r="T3" t="n">
-        <v>6.873856544494629</v>
+        <v>1.551671630295459e-05</v>
       </c>
       <c r="U3" t="n">
-        <v>5.204483032226562</v>
+        <v>2.921883424278349e-05</v>
       </c>
       <c r="V3" t="n">
-        <v>6.632120609283447</v>
+        <v>3.211889998055995e-05</v>
       </c>
       <c r="W3" t="n">
-        <v>4.60166072845459</v>
+        <v>1.66432667647598e-09</v>
       </c>
       <c r="X3" t="n">
-        <v>6.218491077423096</v>
+        <v>0.0001709639182081446</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.001210002461448312</v>
+        <v>0.002281186869367957</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.9506756067276</v>
+        <v>4.164793426753022e-05</v>
       </c>
       <c r="B4" t="n">
-        <v>0.004224009811878204</v>
+        <v>0.000873119046445936</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01214164029806852</v>
+        <v>9.952799695511771e-10</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01354831922799349</v>
+        <v>2.023156639552326e-06</v>
       </c>
       <c r="E4" t="n">
-        <v>3.908854484558105</v>
+        <v>5.997534913149138e-08</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00608730036765337</v>
+        <v>4.433336653164588e-05</v>
       </c>
       <c r="G4" t="n">
-        <v>2.115115165710449</v>
+        <v>0.0004010562843177468</v>
       </c>
       <c r="H4" t="n">
-        <v>8.032851219177246</v>
+        <v>6.594645321200422e-18</v>
       </c>
       <c r="I4" t="n">
-        <v>4.617366790771484</v>
+        <v>0.002083619823679328</v>
       </c>
       <c r="J4" t="n">
-        <v>1.840412259101868</v>
+        <v>4.361839091870934e-05</v>
       </c>
       <c r="K4" t="n">
-        <v>0.003356289118528366</v>
+        <v>4.966978041642066e-18</v>
       </c>
       <c r="L4" t="n">
-        <v>4.469799518585205</v>
+        <v>1.273284169656108e-06</v>
       </c>
       <c r="M4" t="n">
-        <v>5.621973991394043</v>
+        <v>0.01062809582799673</v>
       </c>
       <c r="N4" t="n">
-        <v>0.621628999710083</v>
+        <v>7.687747129896385e-18</v>
       </c>
       <c r="O4" t="n">
-        <v>2.20595383644104</v>
+        <v>0.000277571874903515</v>
       </c>
       <c r="P4" t="n">
-        <v>1.223170399665833</v>
+        <v>8.418908947760428e-08</v>
       </c>
       <c r="Q4" t="n">
-        <v>4.591441631317139</v>
+        <v>1.199122380057815e-05</v>
       </c>
       <c r="R4" t="n">
-        <v>3.292394399642944</v>
+        <v>8.10360045733205e-09</v>
       </c>
       <c r="S4" t="n">
-        <v>0.004453139379620552</v>
+        <v>0.0001946452393895015</v>
       </c>
       <c r="T4" t="n">
-        <v>0.009770682081580162</v>
+        <v>0.0002477207162883133</v>
       </c>
       <c r="U4" t="n">
-        <v>0.2070891261100769</v>
+        <v>0.0001232908689416945</v>
       </c>
       <c r="V4" t="n">
-        <v>0.684496283531189</v>
+        <v>4.831540536542889e-07</v>
       </c>
       <c r="W4" t="n">
-        <v>5.382015228271484</v>
+        <v>1.573590964198956e-07</v>
       </c>
       <c r="X4" t="n">
-        <v>0.8915483951568604</v>
+        <v>0.0006239789072424173</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.002153449924662709</v>
+        <v>0.001610737759619951</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.461140275001526</v>
+        <v>0.0004995528142899275</v>
       </c>
       <c r="B5" t="n">
-        <v>0.004304415080696344</v>
+        <v>0.0007081272779032588</v>
       </c>
       <c r="C5" t="n">
-        <v>2.584566593170166</v>
+        <v>0.001123439986258745</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0201956033706665</v>
+        <v>9.34303159283445e-08</v>
       </c>
       <c r="E5" t="n">
-        <v>3.477282285690308</v>
+        <v>0.0001596799120306969</v>
       </c>
       <c r="F5" t="n">
-        <v>0.003808443201705813</v>
+        <v>1.792307898540457e-06</v>
       </c>
       <c r="G5" t="n">
-        <v>0.003639432601630688</v>
+        <v>0.0003022235177922994</v>
       </c>
       <c r="H5" t="n">
-        <v>6.121278762817383</v>
+        <v>3.338568532740283e-08</v>
       </c>
       <c r="I5" t="n">
-        <v>0.003637688234448433</v>
+        <v>2.622188367240597e-05</v>
       </c>
       <c r="J5" t="n">
-        <v>3.464127063751221</v>
+        <v>1.333777709078277e-05</v>
       </c>
       <c r="K5" t="n">
-        <v>0.00824928842484951</v>
+        <v>1.415430270606236e-17</v>
       </c>
       <c r="L5" t="n">
-        <v>0.003916628658771515</v>
+        <v>5.402661145126331e-07</v>
       </c>
       <c r="M5" t="n">
-        <v>4.584489345550537</v>
+        <v>0.009919251315295696</v>
       </c>
       <c r="N5" t="n">
-        <v>1.48308253288269</v>
+        <v>4.544984903830993e-17</v>
       </c>
       <c r="O5" t="n">
-        <v>4.691103935241699</v>
+        <v>9.185194357996807e-05</v>
       </c>
       <c r="P5" t="n">
-        <v>2.149705648422241</v>
+        <v>2.218024377498296e-07</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.002888125367462635</v>
+        <v>3.165545786032453e-05</v>
       </c>
       <c r="R5" t="n">
-        <v>4.577437877655029</v>
+        <v>1.02748308563605e-05</v>
       </c>
       <c r="S5" t="n">
-        <v>5.123556137084961</v>
+        <v>0.0001060937429429032</v>
       </c>
       <c r="T5" t="n">
-        <v>2.871350526809692</v>
+        <v>7.973251194925979e-05</v>
       </c>
       <c r="U5" t="n">
-        <v>3.953562259674072</v>
+        <v>0.0002137173141818494</v>
       </c>
       <c r="V5" t="n">
-        <v>4.243963718414307</v>
+        <v>1.540154698886909e-05</v>
       </c>
       <c r="W5" t="n">
-        <v>0.003135476727038622</v>
+        <v>3.28467604049365e-06</v>
       </c>
       <c r="X5" t="n">
-        <v>0.5569941997528076</v>
+        <v>0.0005501061677932739</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.00924244336783886</v>
+        <v>0.003062946023419499</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3.410658597946167</v>
+        <v>0.0001661850401433185</v>
       </c>
       <c r="B6" t="n">
-        <v>0.5193859934806824</v>
+        <v>0.0009311214089393616</v>
       </c>
       <c r="C6" t="n">
-        <v>3.805002689361572</v>
+        <v>1.177775210692289e-08</v>
       </c>
       <c r="D6" t="n">
-        <v>6.188418388366699</v>
+        <v>8.150353636438012e-08</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03429876640439034</v>
+        <v>0.005228939466178417</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2813860177993774</v>
+        <v>6.134509078492556e-08</v>
       </c>
       <c r="G6" t="n">
-        <v>5.831648349761963</v>
+        <v>0.0002242642513010651</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5426952242851257</v>
+        <v>1.149991734350726e-17</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01319483108818531</v>
+        <v>8.601014997111633e-06</v>
       </c>
       <c r="J6" t="n">
-        <v>1.831418633460999</v>
+        <v>0.0001464478846173733</v>
       </c>
       <c r="K6" t="n">
-        <v>5.579594612121582</v>
+        <v>7.411131809931248e-05</v>
       </c>
       <c r="L6" t="n">
-        <v>0.00465824268758297</v>
+        <v>1.303019899518852e-17</v>
       </c>
       <c r="M6" t="n">
-        <v>0.004029155243188143</v>
+        <v>0.006362977437674999</v>
       </c>
       <c r="N6" t="n">
-        <v>5.427706241607666</v>
+        <v>6.923304858083054e-18</v>
       </c>
       <c r="O6" t="n">
-        <v>1.787075757980347</v>
+        <v>5.276109277474461e-06</v>
       </c>
       <c r="P6" t="n">
-        <v>0.003378417575731874</v>
+        <v>3.476714055539176e-11</v>
       </c>
       <c r="Q6" t="n">
-        <v>5.225881576538086</v>
+        <v>8.808006555227621e-07</v>
       </c>
       <c r="R6" t="n">
-        <v>0.007809703703969717</v>
+        <v>5.007824256608728e-06</v>
       </c>
       <c r="S6" t="n">
-        <v>0.5318001508712769</v>
+        <v>0.0002270957047585398</v>
       </c>
       <c r="T6" t="n">
-        <v>0.01222683489322662</v>
+        <v>2.061329951175139e-08</v>
       </c>
       <c r="U6" t="n">
-        <v>1.937697172164917</v>
+        <v>7.879411495269822e-18</v>
       </c>
       <c r="V6" t="n">
-        <v>0.004065602086484432</v>
+        <v>3.971583240058862e-08</v>
       </c>
       <c r="W6" t="n">
-        <v>1.937944531440735</v>
+        <v>3.122039800018683e-07</v>
       </c>
       <c r="X6" t="n">
-        <v>0.0103471614420414</v>
+        <v>2.542059618360071e-11</v>
       </c>
       <c r="Y6" t="n">
-        <v>5.803413391113281</v>
+        <v>0.001226022955961525</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2.844599008560181</v>
+        <v>0.0003369326295796782</v>
       </c>
       <c r="B7" t="n">
-        <v>4.741164207458496</v>
+        <v>0.0007517669582739472</v>
       </c>
       <c r="C7" t="n">
-        <v>0.002243695314973593</v>
+        <v>0.0001107530333683826</v>
       </c>
       <c r="D7" t="n">
-        <v>1.268503427505493</v>
+        <v>1.853537838769626e-07</v>
       </c>
       <c r="E7" t="n">
-        <v>8.398907661437988</v>
+        <v>4.447271422918115e-19</v>
       </c>
       <c r="F7" t="n">
-        <v>4.01053524017334</v>
+        <v>1.81109285790626e-07</v>
       </c>
       <c r="G7" t="n">
-        <v>0.005037608556449413</v>
+        <v>0.0002258610766148195</v>
       </c>
       <c r="H7" t="n">
-        <v>2.781199932098389</v>
+        <v>1.445805963973184e-16</v>
       </c>
       <c r="I7" t="n">
-        <v>0.001711501041427255</v>
+        <v>0.000140322299557738</v>
       </c>
       <c r="J7" t="n">
-        <v>0.001031458843499422</v>
+        <v>0.001625792006962001</v>
       </c>
       <c r="K7" t="n">
-        <v>2.740577936172485</v>
+        <v>3.267081183366827e-08</v>
       </c>
       <c r="L7" t="n">
-        <v>1.787148714065552</v>
+        <v>4.314128432270081e-07</v>
       </c>
       <c r="M7" t="n">
-        <v>0.4003611207008362</v>
+        <v>0.009886804036796093</v>
       </c>
       <c r="N7" t="n">
-        <v>0.005779871717095375</v>
+        <v>1.036427131980198e-16</v>
       </c>
       <c r="O7" t="n">
-        <v>0.001129458658397198</v>
+        <v>4.240775524522178e-05</v>
       </c>
       <c r="P7" t="n">
-        <v>1.951138734817505</v>
+        <v>3.262393022396282e-07</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.03499886021018028</v>
+        <v>1.620000148250256e-05</v>
       </c>
       <c r="R7" t="n">
-        <v>1.159641742706299</v>
+        <v>6.430234122944967e-08</v>
       </c>
       <c r="S7" t="n">
-        <v>6.422484397888184</v>
+        <v>6.90019951434806e-05</v>
       </c>
       <c r="T7" t="n">
-        <v>0.007131356745958328</v>
+        <v>9.146166121354327e-05</v>
       </c>
       <c r="U7" t="n">
-        <v>5.555715084075928</v>
+        <v>0.0002531820500735193</v>
       </c>
       <c r="V7" t="n">
-        <v>1.059916973114014</v>
+        <v>7.109832222340629e-05</v>
       </c>
       <c r="W7" t="n">
-        <v>0.130394920706749</v>
+        <v>5.794519438495627e-06</v>
       </c>
       <c r="X7" t="n">
-        <v>0.008469589985907078</v>
+        <v>0.0006738266092725098</v>
       </c>
       <c r="Y7" t="n">
-        <v>5.590366363525391</v>
+        <v>0.002702496480196714</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.498386859893799</v>
+        <v>0.0001596811489434913</v>
       </c>
       <c r="B8" t="n">
-        <v>0.233984500169754</v>
+        <v>0.0007996290805749595</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3373751044273376</v>
+        <v>2.362860663287494e-15</v>
       </c>
       <c r="D8" t="n">
-        <v>4.206531524658203</v>
+        <v>1.256528776139021e-06</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0001562673423904926</v>
+        <v>0.0003429708594921976</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01127286721020937</v>
+        <v>1.098644816011074e-06</v>
       </c>
       <c r="G8" t="n">
-        <v>1.683412313461304</v>
+        <v>5.37697305844631e-05</v>
       </c>
       <c r="H8" t="n">
-        <v>0.001065192511305213</v>
+        <v>3.238285728457413e-07</v>
       </c>
       <c r="I8" t="n">
-        <v>5.496126651763916</v>
+        <v>9.783330464205165e-17</v>
       </c>
       <c r="J8" t="n">
-        <v>0.001083079841919243</v>
+        <v>0.0003655441978480667</v>
       </c>
       <c r="K8" t="n">
-        <v>5.948645114898682</v>
+        <v>1.69156464835396e-06</v>
       </c>
       <c r="L8" t="n">
-        <v>5.852470874786377</v>
+        <v>7.461642326234141e-07</v>
       </c>
       <c r="M8" t="n">
-        <v>0.001966696232557297</v>
+        <v>0.01067871227860451</v>
       </c>
       <c r="N8" t="n">
-        <v>0.2667432427406311</v>
+        <v>5.583078705483812e-17</v>
       </c>
       <c r="O8" t="n">
-        <v>0.0009038528660312295</v>
+        <v>6.104653584770858e-05</v>
       </c>
       <c r="P8" t="n">
-        <v>0.4684150516986847</v>
+        <v>6.301378107309574e-06</v>
       </c>
       <c r="Q8" t="n">
-        <v>2.199663400650024</v>
+        <v>1.820612283154333e-07</v>
       </c>
       <c r="R8" t="n">
-        <v>8.177361488342285</v>
+        <v>6.159193435451016e-05</v>
       </c>
       <c r="S8" t="n">
-        <v>0.07305580377578735</v>
+        <v>0.0003235218173358589</v>
       </c>
       <c r="T8" t="n">
-        <v>0.1000940054655075</v>
+        <v>0.0002318381448276341</v>
       </c>
       <c r="U8" t="n">
-        <v>0.886012852191925</v>
+        <v>1.43867546285037e-05</v>
       </c>
       <c r="V8" t="n">
-        <v>0.0004968990106135607</v>
+        <v>0.001272225752472878</v>
       </c>
       <c r="W8" t="n">
-        <v>5.005722999572754</v>
+        <v>2.197476169385482e-05</v>
       </c>
       <c r="X8" t="n">
-        <v>5.099513530731201</v>
+        <v>0.0007041794015094638</v>
       </c>
       <c r="Y8" t="n">
-        <v>4.210269927978516</v>
+        <v>0.002106880536302924</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.005901766940951347</v>
+        <v>0.0002469881437718868</v>
       </c>
       <c r="B9" t="n">
-        <v>4.256443500518799</v>
+        <v>0.000550118216779083</v>
       </c>
       <c r="C9" t="n">
-        <v>5.195938110351562</v>
+        <v>1.912545667437371e-05</v>
       </c>
       <c r="D9" t="n">
-        <v>0.006182674318552017</v>
+        <v>1.698408937045315e-06</v>
       </c>
       <c r="E9" t="n">
-        <v>0.001698993495665491</v>
+        <v>1.843013164124697e-17</v>
       </c>
       <c r="F9" t="n">
-        <v>3.949512004852295</v>
+        <v>4.558618513783586e-07</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3545295894145966</v>
+        <v>0.0002102444559568539</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8364130854606628</v>
+        <v>1.928758540985821e-17</v>
       </c>
       <c r="I9" t="n">
-        <v>0.09276384860277176</v>
+        <v>0.0001744547043927014</v>
       </c>
       <c r="J9" t="n">
-        <v>6.77872896194458</v>
+        <v>4.910009374725632e-05</v>
       </c>
       <c r="K9" t="n">
-        <v>0.01233084686100483</v>
+        <v>1.374942826259939e-06</v>
       </c>
       <c r="L9" t="n">
-        <v>0.004123758990317583</v>
+        <v>8.712789281162259e-07</v>
       </c>
       <c r="M9" t="n">
-        <v>0.003267535008490086</v>
+        <v>0.009681799449026585</v>
       </c>
       <c r="N9" t="n">
-        <v>5.680654525756836</v>
+        <v>4.515666451876399e-10</v>
       </c>
       <c r="O9" t="n">
-        <v>7.149709224700928</v>
+        <v>0.0009832425275817513</v>
       </c>
       <c r="P9" t="n">
-        <v>4.894673347473145</v>
+        <v>1.136164442527843e-07</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.06682708114385605</v>
+        <v>0.0001140882959589362</v>
       </c>
       <c r="R9" t="n">
-        <v>0.007031361106783152</v>
+        <v>3.828645500743336e-17</v>
       </c>
       <c r="S9" t="n">
-        <v>0.008566330187022686</v>
+        <v>6.878614658489823e-05</v>
       </c>
       <c r="T9" t="n">
-        <v>0.3613593876361847</v>
+        <v>9.424791642231867e-06</v>
       </c>
       <c r="U9" t="n">
-        <v>0.004120903089642525</v>
+        <v>0.0003191560972481966</v>
       </c>
       <c r="V9" t="n">
-        <v>7.000304222106934</v>
+        <v>0.0002470989711582661</v>
       </c>
       <c r="W9" t="n">
-        <v>2.666243314743042</v>
+        <v>7.276165888470132e-06</v>
       </c>
       <c r="X9" t="n">
-        <v>0.01006762124598026</v>
+        <v>1.400855489919195e-05</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.003580531338229775</v>
+        <v>0.00296163116581738</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3.255012989044189</v>
+        <v>0.0004361461324151605</v>
       </c>
       <c r="B10" t="n">
-        <v>5.15381908416748</v>
+        <v>0.0008663510670885444</v>
       </c>
       <c r="C10" t="n">
-        <v>2.272378206253052</v>
+        <v>4.186919341009343e-06</v>
       </c>
       <c r="D10" t="n">
-        <v>0.003712342819198966</v>
+        <v>2.181029709863013e-14</v>
       </c>
       <c r="E10" t="n">
-        <v>2.640583992004395</v>
+        <v>3.28313014380421e-17</v>
       </c>
       <c r="F10" t="n">
-        <v>4.243880748748779</v>
+        <v>0.001906165038235486</v>
       </c>
       <c r="G10" t="n">
-        <v>0.004041530191898346</v>
+        <v>0.000521318637765944</v>
       </c>
       <c r="H10" t="n">
-        <v>0.007993529550731182</v>
+        <v>3.800306954701759e-17</v>
       </c>
       <c r="I10" t="n">
-        <v>4.409947872161865</v>
+        <v>0.0002027807786362246</v>
       </c>
       <c r="J10" t="n">
-        <v>2.664298295974731</v>
+        <v>0.0003878700081259012</v>
       </c>
       <c r="K10" t="n">
-        <v>0.004182351287454367</v>
+        <v>3.023836541160563e-07</v>
       </c>
       <c r="L10" t="n">
-        <v>4.112948417663574</v>
+        <v>2.357251167741968e-17</v>
       </c>
       <c r="M10" t="n">
-        <v>5.114810943603516</v>
+        <v>0.01354031451046467</v>
       </c>
       <c r="N10" t="n">
-        <v>0.004202362149953842</v>
+        <v>4.912015529532612e-17</v>
       </c>
       <c r="O10" t="n">
-        <v>1.058089256286621</v>
+        <v>4.045211881020805e-07</v>
       </c>
       <c r="P10" t="n">
-        <v>0.4905550181865692</v>
+        <v>6.320616100693243e-17</v>
       </c>
       <c r="Q10" t="n">
-        <v>3.316354751586914</v>
+        <v>0.000174307293491438</v>
       </c>
       <c r="R10" t="n">
-        <v>0.002530722878873348</v>
+        <v>5.480202958096925e-07</v>
       </c>
       <c r="S10" t="n">
-        <v>6.137276649475098</v>
+        <v>0.0002562867302913219</v>
       </c>
       <c r="T10" t="n">
-        <v>0.643217146396637</v>
+        <v>0.0002257677115267143</v>
       </c>
       <c r="U10" t="n">
-        <v>2.728050231933594</v>
+        <v>0.0002562968293204904</v>
       </c>
       <c r="V10" t="n">
-        <v>0.002977384487167001</v>
+        <v>7.58857058826834e-05</v>
       </c>
       <c r="W10" t="n">
-        <v>1.678724646568298</v>
+        <v>4.04053116653813e-06</v>
       </c>
       <c r="X10" t="n">
-        <v>1.100385785102844</v>
+        <v>0.0003391627687960863</v>
       </c>
       <c r="Y10" t="n">
-        <v>1.058057188987732</v>
+        <v>0.003512072376906872</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4.212934494018555</v>
+        <v>0.0002580983273219317</v>
       </c>
       <c r="B11" t="n">
-        <v>2.952179431915283</v>
+        <v>0.0007403444615192711</v>
       </c>
       <c r="C11" t="n">
-        <v>5.61153507232666</v>
+        <v>5.471041731652804e-06</v>
       </c>
       <c r="D11" t="n">
-        <v>3.482506990432739</v>
+        <v>2.182753178203711e-06</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0003373771905899048</v>
+        <v>0.002939575584605336</v>
       </c>
       <c r="F11" t="n">
-        <v>3.166513681411743</v>
+        <v>3.47649847753928e-06</v>
       </c>
       <c r="G11" t="n">
-        <v>3.423604488372803</v>
+        <v>0.0001829219982028008</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0001673406222835183</v>
+        <v>2.422149442497163e-18</v>
       </c>
       <c r="I11" t="n">
-        <v>0.04144493117928505</v>
+        <v>0.0001211178459925577</v>
       </c>
       <c r="J11" t="n">
-        <v>2.198819160461426</v>
+        <v>9.777095328900032e-06</v>
       </c>
       <c r="K11" t="n">
-        <v>0.00232517090626061</v>
+        <v>3.242481398046948e-06</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0002239847090095282</v>
+        <v>5.129232594214272e-09</v>
       </c>
       <c r="M11" t="n">
-        <v>0.001565230544656515</v>
+        <v>0.009115278720855713</v>
       </c>
       <c r="N11" t="n">
-        <v>4.012048721313477</v>
+        <v>9.80828915026385e-18</v>
       </c>
       <c r="O11" t="n">
-        <v>2.243364334106445</v>
+        <v>3.097480374100769e-18</v>
       </c>
       <c r="P11" t="n">
-        <v>8.73178768157959</v>
+        <v>9.952897380571812e-05</v>
       </c>
       <c r="Q11" t="n">
-        <v>2.383157253265381</v>
+        <v>3.237030614400283e-05</v>
       </c>
       <c r="R11" t="n">
-        <v>0.0007974395994096994</v>
+        <v>2.22148855755222e-06</v>
       </c>
       <c r="S11" t="n">
-        <v>0.0002751208376139402</v>
+        <v>0.0003115073195658624</v>
       </c>
       <c r="T11" t="n">
-        <v>1.319719552993774</v>
+        <v>1.167744630947709e-05</v>
       </c>
       <c r="U11" t="n">
-        <v>0.9394583106040955</v>
+        <v>0.000315976794809103</v>
       </c>
       <c r="V11" t="n">
-        <v>0.003731885924935341</v>
+        <v>4.540929876384325e-05</v>
       </c>
       <c r="W11" t="n">
-        <v>0.01734456792473793</v>
+        <v>0.0001954954495886341</v>
       </c>
       <c r="X11" t="n">
-        <v>0.004488531500101089</v>
+        <v>0.002216053893789649</v>
       </c>
       <c r="Y11" t="n">
-        <v>5.287984848022461</v>
+        <v>0.0008682330953888595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>